<commit_message>
Cambios sobre distintos apartados del proyecto.
</commit_message>
<xml_diff>
--- a/INPUT/Resultados/TablaGeneral.xlsx
+++ b/INPUT/Resultados/TablaGeneral.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/549d6ce7d270bfdc/Documentos/TFG_Lucia/GitHub/Automatizacion_PDF_scraping/Automatizacion_PDF_scraping/INPUT/Resultados/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="29" documentId="11_D1069CCD97D9AECF8A160BC4C31CB80A4ECE0692" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{451B098C-25E2-4B22-90D5-7F8EB7C1A85E}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="54">
   <si>
     <t>Número de chip</t>
   </si>
@@ -65,60 +71,6 @@
   </si>
   <si>
     <t>SI/NO fármacos</t>
-  </si>
-  <si>
-    <t>100</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>4</t>
-  </si>
-  <si>
-    <t>5</t>
-  </si>
-  <si>
-    <t>6</t>
-  </si>
-  <si>
-    <t>7</t>
-  </si>
-  <si>
-    <t>8</t>
-  </si>
-  <si>
-    <t>00021</t>
-  </si>
-  <si>
-    <t>00022</t>
-  </si>
-  <si>
-    <t>00023</t>
-  </si>
-  <si>
-    <t>00024</t>
-  </si>
-  <si>
-    <t>00025</t>
-  </si>
-  <si>
-    <t>00026</t>
-  </si>
-  <si>
-    <t>00027</t>
-  </si>
-  <si>
-    <t>00028</t>
-  </si>
-  <si>
-    <t>1234567</t>
   </si>
   <si>
     <t>23B00021-A1</t>
@@ -235,8 +187,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -288,24 +240,33 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -343,7 +304,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -377,6 +338,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -411,9 +373,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -586,14 +549,28 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K15" sqref="K15"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="5" customWidth="1"/>
+    <col min="2" max="2" width="6.28515625" customWidth="1"/>
+    <col min="3" max="3" width="5.28515625" customWidth="1"/>
+    <col min="5" max="5" width="15.140625" customWidth="1"/>
+    <col min="6" max="6" width="4.85546875" customWidth="1"/>
+    <col min="7" max="7" width="12.85546875" customWidth="1"/>
+    <col min="8" max="8" width="17.5703125" customWidth="1"/>
+    <col min="10" max="10" width="16.7109375" customWidth="1"/>
+    <col min="13" max="13" width="14.42578125" customWidth="1"/>
+    <col min="14" max="14" width="15.140625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:18">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -646,48 +623,48 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:18">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="2">
+        <v>100</v>
+      </c>
+      <c r="C2" s="2">
+        <v>1</v>
+      </c>
+      <c r="D2" s="2">
+        <v>21</v>
+      </c>
+      <c r="E2" t="s">
         <v>17</v>
       </c>
-      <c r="C2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D2" t="s">
-        <v>26</v>
-      </c>
-      <c r="E2" t="s">
-        <v>35</v>
-      </c>
-      <c r="F2" t="s">
-        <v>18</v>
+      <c r="F2" s="2">
+        <v>1</v>
       </c>
       <c r="G2" t="s">
-        <v>45</v>
+        <v>27</v>
       </c>
       <c r="H2" t="s">
-        <v>47</v>
+        <v>29</v>
       </c>
       <c r="I2">
         <v>15.1</v>
       </c>
       <c r="J2" t="s">
-        <v>50</v>
+        <v>32</v>
       </c>
       <c r="K2" t="s">
-        <v>58</v>
+        <v>40</v>
       </c>
       <c r="L2">
         <v>1</v>
       </c>
       <c r="M2" t="s">
-        <v>65</v>
+        <v>47</v>
       </c>
       <c r="N2" t="s">
-        <v>71</v>
+        <v>53</v>
       </c>
       <c r="O2">
         <v>6</v>
@@ -702,48 +679,48 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:18">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
-      <c r="B3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="B3" s="2">
+        <v>100</v>
+      </c>
+      <c r="C3" s="2">
+        <v>2</v>
+      </c>
+      <c r="D3" s="2">
+        <v>22</v>
+      </c>
+      <c r="E3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" s="2">
+        <v>1</v>
+      </c>
+      <c r="G3" t="s">
         <v>27</v>
       </c>
-      <c r="E3" t="s">
-        <v>36</v>
-      </c>
-      <c r="F3" t="s">
-        <v>18</v>
-      </c>
-      <c r="G3" t="s">
-        <v>45</v>
-      </c>
       <c r="H3" t="s">
-        <v>47</v>
+        <v>29</v>
       </c>
       <c r="I3">
         <v>15.1</v>
       </c>
       <c r="J3" t="s">
-        <v>51</v>
+        <v>33</v>
       </c>
       <c r="K3" t="s">
-        <v>59</v>
+        <v>41</v>
       </c>
       <c r="L3">
         <v>1</v>
       </c>
       <c r="M3" t="s">
-        <v>66</v>
+        <v>48</v>
       </c>
       <c r="N3" t="s">
-        <v>52</v>
+        <v>34</v>
       </c>
       <c r="O3">
         <v>5</v>
@@ -758,48 +735,48 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:18">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2</v>
       </c>
-      <c r="B4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D4" t="s">
-        <v>28</v>
+      <c r="B4" s="2">
+        <v>100</v>
+      </c>
+      <c r="C4" s="2">
+        <v>3</v>
+      </c>
+      <c r="D4" s="2">
+        <v>23</v>
       </c>
       <c r="E4" t="s">
-        <v>37</v>
-      </c>
-      <c r="F4" t="s">
-        <v>18</v>
+        <v>19</v>
+      </c>
+      <c r="F4" s="2">
+        <v>1</v>
       </c>
       <c r="G4" t="s">
-        <v>45</v>
+        <v>27</v>
       </c>
       <c r="H4" t="s">
-        <v>47</v>
+        <v>29</v>
       </c>
       <c r="I4">
         <v>15.1</v>
       </c>
       <c r="J4" t="s">
-        <v>52</v>
+        <v>34</v>
       </c>
       <c r="K4" t="s">
-        <v>52</v>
+        <v>34</v>
       </c>
       <c r="L4">
         <v>0</v>
       </c>
       <c r="M4" t="s">
-        <v>52</v>
+        <v>34</v>
       </c>
       <c r="N4" t="s">
-        <v>52</v>
+        <v>34</v>
       </c>
       <c r="O4">
         <v>0</v>
@@ -814,48 +791,48 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:18">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>3</v>
       </c>
-      <c r="B5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C5" t="s">
-        <v>21</v>
-      </c>
-      <c r="D5" t="s">
+      <c r="B5" s="2">
+        <v>100</v>
+      </c>
+      <c r="C5" s="2">
+        <v>4</v>
+      </c>
+      <c r="D5" s="2">
+        <v>24</v>
+      </c>
+      <c r="E5" t="s">
+        <v>20</v>
+      </c>
+      <c r="F5" s="2">
+        <v>1</v>
+      </c>
+      <c r="G5" t="s">
+        <v>27</v>
+      </c>
+      <c r="H5" t="s">
         <v>29</v>
-      </c>
-      <c r="E5" t="s">
-        <v>38</v>
-      </c>
-      <c r="F5" t="s">
-        <v>18</v>
-      </c>
-      <c r="G5" t="s">
-        <v>45</v>
-      </c>
-      <c r="H5" t="s">
-        <v>47</v>
       </c>
       <c r="I5">
         <v>15.1</v>
       </c>
       <c r="J5" t="s">
-        <v>53</v>
+        <v>35</v>
       </c>
       <c r="K5" t="s">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="L5">
         <v>2</v>
       </c>
       <c r="M5" t="s">
-        <v>52</v>
+        <v>34</v>
       </c>
       <c r="N5" t="s">
-        <v>52</v>
+        <v>34</v>
       </c>
       <c r="O5">
         <v>0</v>
@@ -870,48 +847,48 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:18">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>4</v>
       </c>
-      <c r="B6" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D6" t="s">
-        <v>30</v>
+      <c r="B6" s="2">
+        <v>100</v>
+      </c>
+      <c r="C6" s="2">
+        <v>5</v>
+      </c>
+      <c r="D6" s="2">
+        <v>25</v>
       </c>
       <c r="E6" t="s">
-        <v>39</v>
-      </c>
-      <c r="F6" t="s">
-        <v>20</v>
+        <v>21</v>
+      </c>
+      <c r="F6" s="2">
+        <v>3</v>
       </c>
       <c r="G6" t="s">
-        <v>45</v>
+        <v>27</v>
       </c>
       <c r="H6" t="s">
-        <v>47</v>
+        <v>29</v>
       </c>
       <c r="I6">
         <v>15.1</v>
       </c>
       <c r="J6" t="s">
-        <v>54</v>
+        <v>36</v>
       </c>
       <c r="K6" t="s">
-        <v>61</v>
+        <v>43</v>
       </c>
       <c r="L6">
         <v>2</v>
       </c>
       <c r="M6" t="s">
-        <v>67</v>
+        <v>49</v>
       </c>
       <c r="N6" t="s">
-        <v>52</v>
+        <v>34</v>
       </c>
       <c r="O6">
         <v>3</v>
@@ -926,48 +903,48 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:18">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>5</v>
       </c>
-      <c r="B7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C7" t="s">
-        <v>23</v>
-      </c>
-      <c r="D7" t="s">
-        <v>31</v>
+      <c r="B7" s="2">
+        <v>100</v>
+      </c>
+      <c r="C7" s="2">
+        <v>6</v>
+      </c>
+      <c r="D7" s="2">
+        <v>26</v>
       </c>
       <c r="E7" t="s">
-        <v>40</v>
-      </c>
-      <c r="F7" t="s">
-        <v>19</v>
+        <v>22</v>
+      </c>
+      <c r="F7" s="2">
+        <v>2</v>
       </c>
       <c r="G7" t="s">
-        <v>45</v>
+        <v>27</v>
       </c>
       <c r="H7" t="s">
-        <v>47</v>
+        <v>29</v>
       </c>
       <c r="I7">
         <v>15.1</v>
       </c>
       <c r="J7" t="s">
-        <v>55</v>
+        <v>37</v>
       </c>
       <c r="K7" t="s">
-        <v>62</v>
+        <v>44</v>
       </c>
       <c r="L7">
         <v>2</v>
       </c>
       <c r="M7" t="s">
-        <v>68</v>
+        <v>50</v>
       </c>
       <c r="N7" t="s">
-        <v>52</v>
+        <v>34</v>
       </c>
       <c r="O7">
         <v>5</v>
@@ -982,48 +959,48 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:18">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>6</v>
       </c>
-      <c r="B8" t="s">
-        <v>17</v>
-      </c>
-      <c r="C8" t="s">
-        <v>24</v>
-      </c>
-      <c r="D8" t="s">
-        <v>32</v>
+      <c r="B8" s="2">
+        <v>100</v>
+      </c>
+      <c r="C8" s="2">
+        <v>7</v>
+      </c>
+      <c r="D8" s="2">
+        <v>27</v>
       </c>
       <c r="E8" t="s">
-        <v>41</v>
-      </c>
-      <c r="F8" t="s">
-        <v>18</v>
+        <v>23</v>
+      </c>
+      <c r="F8" s="2">
+        <v>1</v>
       </c>
       <c r="G8" t="s">
-        <v>45</v>
+        <v>27</v>
       </c>
       <c r="H8" t="s">
-        <v>48</v>
+        <v>30</v>
       </c>
       <c r="I8">
         <v>30</v>
       </c>
       <c r="J8" t="s">
-        <v>56</v>
+        <v>38</v>
       </c>
       <c r="K8" t="s">
-        <v>63</v>
+        <v>45</v>
       </c>
       <c r="L8">
         <v>1</v>
       </c>
       <c r="M8" t="s">
-        <v>69</v>
+        <v>51</v>
       </c>
       <c r="N8" t="s">
-        <v>52</v>
+        <v>34</v>
       </c>
       <c r="O8">
         <v>1</v>
@@ -1038,48 +1015,48 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:18">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>7</v>
       </c>
-      <c r="B9" t="s">
-        <v>17</v>
-      </c>
-      <c r="C9" t="s">
-        <v>25</v>
-      </c>
-      <c r="D9" t="s">
-        <v>33</v>
+      <c r="B9" s="2">
+        <v>100</v>
+      </c>
+      <c r="C9" s="2">
+        <v>8</v>
+      </c>
+      <c r="D9" s="2">
+        <v>28</v>
       </c>
       <c r="E9" t="s">
-        <v>42</v>
-      </c>
-      <c r="F9" t="s">
-        <v>18</v>
+        <v>24</v>
+      </c>
+      <c r="F9" s="2">
+        <v>1</v>
       </c>
       <c r="G9" t="s">
-        <v>45</v>
+        <v>27</v>
       </c>
       <c r="H9" t="s">
-        <v>49</v>
+        <v>31</v>
       </c>
       <c r="I9">
         <v>11</v>
       </c>
       <c r="J9" t="s">
-        <v>57</v>
+        <v>39</v>
       </c>
       <c r="K9" t="s">
-        <v>64</v>
+        <v>46</v>
       </c>
       <c r="L9">
         <v>2</v>
       </c>
       <c r="M9" t="s">
-        <v>70</v>
+        <v>52</v>
       </c>
       <c r="N9" t="s">
-        <v>52</v>
+        <v>34</v>
       </c>
       <c r="O9">
         <v>0</v>
@@ -1094,48 +1071,48 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:18">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>8</v>
       </c>
-      <c r="B10" t="s">
-        <v>17</v>
-      </c>
-      <c r="C10" t="s">
-        <v>18</v>
-      </c>
-      <c r="D10" t="s">
-        <v>34</v>
+      <c r="B10" s="2">
+        <v>100</v>
+      </c>
+      <c r="C10" s="2">
+        <v>1</v>
+      </c>
+      <c r="D10" s="2">
+        <v>1234567</v>
       </c>
       <c r="E10" t="s">
-        <v>43</v>
-      </c>
-      <c r="F10" t="s">
-        <v>18</v>
+        <v>25</v>
+      </c>
+      <c r="F10" s="2">
+        <v>1</v>
       </c>
       <c r="G10" t="s">
-        <v>46</v>
+        <v>28</v>
       </c>
       <c r="H10" t="s">
-        <v>47</v>
+        <v>29</v>
       </c>
       <c r="I10">
         <v>15.1</v>
       </c>
       <c r="J10" t="s">
-        <v>50</v>
+        <v>32</v>
       </c>
       <c r="K10" t="s">
-        <v>58</v>
+        <v>40</v>
       </c>
       <c r="L10">
         <v>1</v>
       </c>
       <c r="M10" t="s">
-        <v>65</v>
+        <v>47</v>
       </c>
       <c r="N10" t="s">
-        <v>71</v>
+        <v>53</v>
       </c>
       <c r="O10">
         <v>6</v>
@@ -1150,48 +1127,48 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:18">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>9</v>
       </c>
-      <c r="B11" t="s">
-        <v>17</v>
-      </c>
-      <c r="C11" t="s">
-        <v>19</v>
-      </c>
-      <c r="D11" t="s">
-        <v>34</v>
+      <c r="B11" s="2">
+        <v>100</v>
+      </c>
+      <c r="C11" s="2">
+        <v>2</v>
+      </c>
+      <c r="D11" s="2">
+        <v>1234567</v>
       </c>
       <c r="E11" t="s">
-        <v>44</v>
-      </c>
-      <c r="F11" t="s">
-        <v>18</v>
+        <v>26</v>
+      </c>
+      <c r="F11" s="2">
+        <v>1</v>
       </c>
       <c r="G11" t="s">
-        <v>46</v>
+        <v>28</v>
       </c>
       <c r="H11" t="s">
-        <v>47</v>
+        <v>29</v>
       </c>
       <c r="I11">
         <v>15.1</v>
       </c>
       <c r="J11" t="s">
-        <v>51</v>
+        <v>33</v>
       </c>
       <c r="K11" t="s">
-        <v>59</v>
+        <v>41</v>
       </c>
       <c r="L11">
         <v>1</v>
       </c>
       <c r="M11" t="s">
-        <v>66</v>
+        <v>48</v>
       </c>
       <c r="N11" t="s">
-        <v>52</v>
+        <v>34</v>
       </c>
       <c r="O11">
         <v>4</v>

</xml_diff>